<commit_message>
fix: openai api, data base
</commit_message>
<xml_diff>
--- a/files/generated_file.xlsx
+++ b/files/generated_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -31,16 +31,7 @@
     <t>nopeacefulll</t>
   </si>
   <si>
-    <t>4/23/2025, 7:45:54 PM</t>
-  </si>
-  <si>
-    <t>eve</t>
-  </si>
-  <si>
-    <t>evvochkaaaaa</t>
-  </si>
-  <si>
-    <t>4/23/2025, 7:48:52 PM</t>
+    <t>2025-05-13 13:02</t>
   </si>
 </sst>
 </file>
@@ -417,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -446,20 +437,6 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>524223430</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>